<commit_message>
master commit add one
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\final450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4CCFA0E8-12E8-4935-AD19-FF3712C2B917}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3EBE6C-B97B-403A-8185-94520C006152}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1355" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1356" uniqueCount="473">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1442,6 +1441,9 @@
   </si>
   <si>
     <t>M58</t>
+  </si>
+  <si>
+    <t>reverse -&gt; add one -&gt; reverse</t>
   </si>
 </sst>
 </file>
@@ -1890,8 +1892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="99" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="A132" zoomScale="99" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B172" sqref="B172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3407,7 +3409,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="21">
+    <row r="145" spans="1:4" ht="21">
       <c r="A145" s="8" t="s">
         <v>134</v>
       </c>
@@ -3418,7 +3420,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="146" spans="1:3" ht="21">
+    <row r="146" spans="1:4" ht="21">
       <c r="A146" s="8" t="s">
         <v>134</v>
       </c>
@@ -3429,18 +3431,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="21">
+    <row r="147" spans="1:4" ht="21">
       <c r="A147" s="8" t="s">
         <v>134</v>
       </c>
       <c r="B147" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="C147" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" ht="21">
+      <c r="C147" s="11" t="s">
+        <v>465</v>
+      </c>
+      <c r="D147" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" ht="21">
       <c r="A148" s="8" t="s">
         <v>134</v>
       </c>
@@ -3451,7 +3456,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="149" spans="1:3" ht="21">
+    <row r="149" spans="1:4" ht="21">
       <c r="A149" s="8" t="s">
         <v>134</v>
       </c>
@@ -3462,7 +3467,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="150" spans="1:3" ht="21">
+    <row r="150" spans="1:4" ht="21">
       <c r="A150" s="8" t="s">
         <v>134</v>
       </c>
@@ -3473,7 +3478,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="151" spans="1:3" ht="21">
+    <row r="151" spans="1:4" ht="21">
       <c r="A151" s="8" t="s">
         <v>134</v>
       </c>
@@ -3484,7 +3489,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="152" spans="1:3" ht="21">
+    <row r="152" spans="1:4" ht="21">
       <c r="A152" s="8" t="s">
         <v>134</v>
       </c>
@@ -3495,7 +3500,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="153" spans="1:3" ht="21">
+    <row r="153" spans="1:4" ht="21">
       <c r="A153" s="8" t="s">
         <v>134</v>
       </c>
@@ -3506,7 +3511,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="154" spans="1:3" ht="21">
+    <row r="154" spans="1:4" ht="21">
       <c r="A154" s="8" t="s">
         <v>134</v>
       </c>
@@ -3517,7 +3522,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="21">
+    <row r="155" spans="1:4" ht="21">
       <c r="A155" s="8" t="s">
         <v>134</v>
       </c>
@@ -3528,7 +3533,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="21">
+    <row r="156" spans="1:4" ht="21">
       <c r="A156" s="8" t="s">
         <v>134</v>
       </c>
@@ -3539,7 +3544,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="21">
+    <row r="157" spans="1:4" ht="21">
       <c r="A157" s="8" t="s">
         <v>134</v>
       </c>
@@ -3550,7 +3555,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="21">
+    <row r="158" spans="1:4" ht="21">
       <c r="A158" s="8" t="s">
         <v>134</v>
       </c>
@@ -3561,7 +3566,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="159" spans="1:3" ht="21">
+    <row r="159" spans="1:4" ht="21">
       <c r="A159" s="8" t="s">
         <v>134</v>
       </c>
@@ -3572,7 +3577,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="160" spans="1:3" ht="21">
+    <row r="160" spans="1:4" ht="21">
       <c r="A160" s="8" t="s">
         <v>134</v>
       </c>

</xml_diff>